<commit_message>
Saving one hot encoder and dataset mean
</commit_message>
<xml_diff>
--- a/HandyML_Trainer/resources/HandyML_Predictor_Template.xlsx
+++ b/HandyML_Trainer/resources/HandyML_Predictor_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8B9BBE-588C-4466-A867-7988EF08A1E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B53FE8-5DA8-44E2-A9C7-389E4C8DF578}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Model path</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Labelencoder file path</t>
+  </si>
+  <si>
+    <t>One hot encoder path</t>
+  </si>
+  <si>
+    <t>Dataset mean path</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,25 +406,35 @@
     </row>
     <row r="3" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>